<commit_message>
organize baseline mapping import
</commit_message>
<xml_diff>
--- a/Replication Package/documentation/rider-audits/baseline-study/codebooks/raw_deidentify.xlsx
+++ b/Replication Package/documentation/rider-audits/baseline-study/codebooks/raw_deidentify.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\rio_vagao_rosa\documentation\rider-audits\baseline-study\codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\rio-safe-space\Replication Package\documentation\rider-audits\baseline-study\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4104FE2D-3F10-409A-A9A5-36FA476CC667}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E064E427-DA03-440C-B88F-C10AC45EE1DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="278">
   <si>
     <t>name</t>
   </si>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2278,6 +2278,9 @@
       </c>
     </row>
     <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
       <c r="C38" t="s">
         <v>20</v>
       </c>

</xml_diff>